<commit_message>
Fix example to make it feasible
</commit_message>
<xml_diff>
--- a/tennis.xlsx
+++ b/tennis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebastian-quintero/github/tennis-scheduler/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3BFFEAB-88F6-1046-912B-415E393A1001}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B7C70E9-5DEB-DC4C-BFE2-89D90F81E523}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="6" xr2:uid="{AA942E56-5CB8-4940-AFE3-FB51AA337CCA}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="3" xr2:uid="{AA942E56-5CB8-4940-AFE3-FB51AA337CCA}"/>
   </bookViews>
   <sheets>
     <sheet name="players" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4718" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4634" uniqueCount="246">
   <si>
     <t>player_id</t>
   </si>
@@ -856,15 +856,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1202,7 +1200,7 @@
   <dimension ref="A1:D103"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B103"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4498,7 +4496,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03AC9C02-052D-FC4F-9BF2-F05552C7E9CD}">
   <dimension ref="A1:C1633"/>
   <sheetViews>
-    <sheetView topLeftCell="A1616" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C1638" sqref="C1638"/>
     </sheetView>
   </sheetViews>
@@ -22480,10 +22478,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50D97DBD-D453-FB49-A851-051BAD27B911}">
-  <dimension ref="A1:B51"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A43" sqref="A43:A51"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -22562,342 +22560,6 @@
       </c>
       <c r="B9" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>157</v>
-      </c>
-      <c r="B10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>157</v>
-      </c>
-      <c r="B11" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>157</v>
-      </c>
-      <c r="B12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>157</v>
-      </c>
-      <c r="B13" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>157</v>
-      </c>
-      <c r="B14" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>157</v>
-      </c>
-      <c r="B15" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>157</v>
-      </c>
-      <c r="B16" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>157</v>
-      </c>
-      <c r="B17" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>172</v>
-      </c>
-      <c r="B18" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>172</v>
-      </c>
-      <c r="B19" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>172</v>
-      </c>
-      <c r="B20" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>172</v>
-      </c>
-      <c r="B21" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>172</v>
-      </c>
-      <c r="B22" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>172</v>
-      </c>
-      <c r="B23" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>172</v>
-      </c>
-      <c r="B24" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>172</v>
-      </c>
-      <c r="B25" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>179</v>
-      </c>
-      <c r="B26" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>179</v>
-      </c>
-      <c r="B27" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>179</v>
-      </c>
-      <c r="B28" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>179</v>
-      </c>
-      <c r="B29" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>179</v>
-      </c>
-      <c r="B30" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>179</v>
-      </c>
-      <c r="B31" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>179</v>
-      </c>
-      <c r="B32" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>179</v>
-      </c>
-      <c r="B33" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>211</v>
-      </c>
-      <c r="B34" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>211</v>
-      </c>
-      <c r="B35" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>211</v>
-      </c>
-      <c r="B36" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>211</v>
-      </c>
-      <c r="B37" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>211</v>
-      </c>
-      <c r="B38" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>211</v>
-      </c>
-      <c r="B39" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>211</v>
-      </c>
-      <c r="B40" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>211</v>
-      </c>
-      <c r="B41" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>211</v>
-      </c>
-      <c r="B42" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>240</v>
-      </c>
-      <c r="B43" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>240</v>
-      </c>
-      <c r="B44" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>240</v>
-      </c>
-      <c r="B45" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>240</v>
-      </c>
-      <c r="B46" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>240</v>
-      </c>
-      <c r="B47" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>240</v>
-      </c>
-      <c r="B48" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>240</v>
-      </c>
-      <c r="B49" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>240</v>
-      </c>
-      <c r="B50" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>240</v>
-      </c>
-      <c r="B51" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -23805,1768 +23467,1767 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85ABF5BC-C2A5-684C-90DC-52EFE8C4DDD7}">
   <dimension ref="A1:E103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="46.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="45.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="10.83203125" style="4"/>
+    <col min="1" max="1" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="46.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="45.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="5" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>144</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>145</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>146</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>147</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>148</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>149</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>150</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>151</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>152</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>153</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E11" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>154</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E12" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>155</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E13" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>156</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="E14" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>157</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="E15" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="4" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>158</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E16" s="5" t="s">
+      <c r="E16" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="s">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>159</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="E17" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>160</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="E18" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>161</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C19" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D19" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E19" s="5" t="s">
+      <c r="E19" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="4" t="s">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>162</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="D20" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E20" s="5" t="s">
+      <c r="E20" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="4" t="s">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>163</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="D21" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E21" s="5" t="s">
+      <c r="E21" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="4" t="s">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
         <v>164</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D22" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E22" s="5" t="s">
+      <c r="E22" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="4" t="s">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>165</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="C23" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D23" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E23" s="5" t="s">
+      <c r="E23" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="24" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="4" t="s">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>166</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="C24" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="D24" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E24" s="5" t="s">
+      <c r="E24" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="4" t="s">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
         <v>167</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B25" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="C25" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="D25" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E25" s="5" t="s">
+      <c r="E25" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="4" t="s">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
         <v>168</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B26" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C26" s="5" t="s">
+      <c r="C26" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="D26" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E26" s="5" t="s">
+      <c r="E26" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="4" t="s">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
         <v>169</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B27" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C27" s="5" t="s">
+      <c r="C27" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="D27" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E27" s="5" t="s">
+      <c r="E27" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="28" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="4" t="s">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>170</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B28" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="C28" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="D28" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E28" s="5" t="s">
+      <c r="E28" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="29" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="4" t="s">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>171</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B29" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="C29" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D29" s="5" t="s">
+      <c r="D29" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E29" s="5" t="s">
+      <c r="E29" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="30" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="4" t="s">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
         <v>172</v>
       </c>
-      <c r="B30" s="5" t="s">
+      <c r="B30" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C30" s="5" t="s">
+      <c r="C30" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D30" s="5" t="s">
+      <c r="D30" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E30" s="5" t="s">
+      <c r="E30" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="31" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="4" t="s">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
         <v>173</v>
       </c>
-      <c r="B31" s="5" t="s">
+      <c r="B31" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C31" s="5" t="s">
+      <c r="C31" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D31" s="5" t="s">
+      <c r="D31" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E31" s="5" t="s">
+      <c r="E31" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="32" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="4" t="s">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
         <v>174</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="B32" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C32" s="5" t="s">
+      <c r="C32" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D32" s="5" t="s">
+      <c r="D32" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E32" s="5" t="s">
+      <c r="E32" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="33" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="4" t="s">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
         <v>175</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="B33" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C33" s="5" t="s">
+      <c r="C33" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D33" s="5" t="s">
+      <c r="D33" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E33" s="5" t="s">
+      <c r="E33" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="34" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="4" t="s">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
         <v>176</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="B34" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C34" s="5" t="s">
+      <c r="C34" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D34" s="5" t="s">
+      <c r="D34" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E34" s="5" t="s">
+      <c r="E34" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="35" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="4" t="s">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
         <v>177</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="B35" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C35" s="5" t="s">
+      <c r="C35" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D35" s="5" t="s">
+      <c r="D35" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E35" s="5" t="s">
+      <c r="E35" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="36" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="4" t="s">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
         <v>178</v>
       </c>
-      <c r="B36" s="5" t="s">
+      <c r="B36" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C36" s="5" t="s">
+      <c r="C36" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D36" s="5" t="s">
+      <c r="D36" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E36" s="5" t="s">
+      <c r="E36" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="37" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="4" t="s">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
         <v>179</v>
       </c>
-      <c r="B37" s="5" t="s">
+      <c r="B37" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C37" s="5" t="s">
+      <c r="C37" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D37" s="5" t="s">
+      <c r="D37" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E37" s="5" t="s">
+      <c r="E37" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="38" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="4" t="s">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
         <v>180</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="B38" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C38" s="5" t="s">
+      <c r="C38" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D38" s="5" t="s">
+      <c r="D38" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E38" s="5" t="s">
+      <c r="E38" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="39" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="4" t="s">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
         <v>181</v>
       </c>
-      <c r="B39" s="5" t="s">
+      <c r="B39" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C39" s="5" t="s">
+      <c r="C39" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D39" s="5" t="s">
+      <c r="D39" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E39" s="5" t="s">
+      <c r="E39" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="40" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="4" t="s">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
         <v>182</v>
       </c>
-      <c r="B40" s="5" t="s">
+      <c r="B40" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C40" s="5" t="s">
+      <c r="C40" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D40" s="5" t="s">
+      <c r="D40" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E40" s="5" t="s">
+      <c r="E40" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="41" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="4" t="s">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
         <v>183</v>
       </c>
-      <c r="B41" s="5" t="s">
+      <c r="B41" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C41" s="5" t="s">
+      <c r="C41" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D41" s="5" t="s">
+      <c r="D41" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E41" s="5" t="s">
+      <c r="E41" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="4" t="s">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
         <v>184</v>
       </c>
-      <c r="B42" s="5" t="s">
+      <c r="B42" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C42" s="5" t="s">
+      <c r="C42" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D42" s="5" t="s">
+      <c r="D42" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E42" s="5" t="s">
+      <c r="E42" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="4" t="s">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
         <v>185</v>
       </c>
-      <c r="B43" s="5" t="s">
+      <c r="B43" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C43" s="5" t="s">
+      <c r="C43" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D43" s="5" t="s">
+      <c r="D43" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E43" s="5" t="s">
+      <c r="E43" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="44" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="4" t="s">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
         <v>186</v>
       </c>
-      <c r="B44" s="5" t="s">
+      <c r="B44" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C44" s="5" t="s">
+      <c r="C44" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D44" s="5" t="s">
+      <c r="D44" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E44" s="5" t="s">
+      <c r="E44" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="45" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="4" t="s">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
         <v>187</v>
       </c>
-      <c r="B45" s="5" t="s">
+      <c r="B45" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C45" s="5" t="s">
+      <c r="C45" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D45" s="5" t="s">
+      <c r="D45" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E45" s="5" t="s">
+      <c r="E45" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="46" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="4" t="s">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
         <v>188</v>
       </c>
-      <c r="B46" s="5" t="s">
+      <c r="B46" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C46" s="5" t="s">
+      <c r="C46" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D46" s="5" t="s">
+      <c r="D46" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E46" s="5" t="s">
+      <c r="E46" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="47" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="4" t="s">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
         <v>189</v>
       </c>
-      <c r="B47" s="5" t="s">
+      <c r="B47" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C47" s="5" t="s">
+      <c r="C47" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D47" s="5" t="s">
+      <c r="D47" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E47" s="5" t="s">
+      <c r="E47" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="48" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="4" t="s">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
         <v>190</v>
       </c>
-      <c r="B48" s="5" t="s">
+      <c r="B48" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C48" s="5" t="s">
+      <c r="C48" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D48" s="5" t="s">
+      <c r="D48" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E48" s="5" t="s">
+      <c r="E48" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="49" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="4" t="s">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
         <v>191</v>
       </c>
-      <c r="B49" s="5" t="s">
+      <c r="B49" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C49" s="5" t="s">
+      <c r="C49" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D49" s="5" t="s">
+      <c r="D49" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E49" s="5" t="s">
+      <c r="E49" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="50" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="4" t="s">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
         <v>192</v>
       </c>
-      <c r="B50" s="5" t="s">
+      <c r="B50" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C50" s="5" t="s">
+      <c r="C50" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D50" s="5" t="s">
+      <c r="D50" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E50" s="5" t="s">
+      <c r="E50" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="51" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="4" t="s">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
         <v>193</v>
       </c>
-      <c r="B51" s="5" t="s">
+      <c r="B51" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C51" s="5" t="s">
+      <c r="C51" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D51" s="5" t="s">
+      <c r="D51" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E51" s="5" t="s">
+      <c r="E51" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="52" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="4" t="s">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
         <v>194</v>
       </c>
-      <c r="B52" s="5" t="s">
+      <c r="B52" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C52" s="5" t="s">
+      <c r="C52" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D52" s="5" t="s">
+      <c r="D52" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E52" s="5" t="s">
+      <c r="E52" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="53" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="4" t="s">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
         <v>195</v>
       </c>
-      <c r="B53" s="5" t="s">
+      <c r="B53" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C53" s="5" t="s">
+      <c r="C53" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D53" s="5" t="s">
+      <c r="D53" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E53" s="5" t="s">
+      <c r="E53" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="54" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="4" t="s">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
         <v>196</v>
       </c>
-      <c r="B54" s="5" t="s">
+      <c r="B54" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C54" s="5" t="s">
+      <c r="C54" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D54" s="5" t="s">
+      <c r="D54" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E54" s="5" t="s">
+      <c r="E54" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="55" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="4" t="s">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
         <v>197</v>
       </c>
-      <c r="B55" s="5" t="s">
+      <c r="B55" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C55" s="5" t="s">
+      <c r="C55" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D55" s="5" t="s">
+      <c r="D55" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E55" s="5" t="s">
+      <c r="E55" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="56" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="4" t="s">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
         <v>198</v>
       </c>
-      <c r="B56" s="5" t="s">
+      <c r="B56" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C56" s="5" t="s">
+      <c r="C56" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D56" s="5" t="s">
+      <c r="D56" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E56" s="5" t="s">
+      <c r="E56" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="57" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="4" t="s">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
         <v>199</v>
       </c>
-      <c r="B57" s="5" t="s">
+      <c r="B57" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C57" s="5" t="s">
+      <c r="C57" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D57" s="5" t="s">
+      <c r="D57" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E57" s="5" t="s">
+      <c r="E57" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="58" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="4" t="s">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
         <v>200</v>
       </c>
-      <c r="B58" s="5" t="s">
+      <c r="B58" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C58" s="5" t="s">
+      <c r="C58" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D58" s="5" t="s">
+      <c r="D58" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E58" s="5" t="s">
+      <c r="E58" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="59" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="4" t="s">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
         <v>201</v>
       </c>
-      <c r="B59" s="5" t="s">
+      <c r="B59" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C59" s="5" t="s">
+      <c r="C59" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D59" s="5" t="s">
+      <c r="D59" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E59" s="5" t="s">
+      <c r="E59" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="60" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="4" t="s">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
         <v>202</v>
       </c>
-      <c r="B60" s="5" t="s">
+      <c r="B60" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C60" s="5" t="s">
+      <c r="C60" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D60" s="5" t="s">
+      <c r="D60" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E60" s="5" t="s">
+      <c r="E60" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="61" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="4" t="s">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
         <v>203</v>
       </c>
-      <c r="B61" s="5" t="s">
+      <c r="B61" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C61" s="5" t="s">
+      <c r="C61" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D61" s="5" t="s">
+      <c r="D61" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E61" s="5" t="s">
+      <c r="E61" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="62" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="4" t="s">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
         <v>204</v>
       </c>
-      <c r="B62" s="5" t="s">
+      <c r="B62" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C62" s="5" t="s">
+      <c r="C62" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D62" s="5" t="s">
+      <c r="D62" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E62" s="5" t="s">
+      <c r="E62" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="63" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="4" t="s">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
         <v>205</v>
       </c>
-      <c r="B63" s="5" t="s">
+      <c r="B63" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C63" s="5" t="s">
+      <c r="C63" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D63" s="5" t="s">
+      <c r="D63" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E63" s="5" t="s">
+      <c r="E63" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="64" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="4" t="s">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
         <v>206</v>
       </c>
-      <c r="B64" s="5" t="s">
+      <c r="B64" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C64" s="5" t="s">
+      <c r="C64" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D64" s="5" t="s">
+      <c r="D64" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E64" s="5" t="s">
+      <c r="E64" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="65" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="4" t="s">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
         <v>207</v>
       </c>
-      <c r="B65" s="5" t="s">
+      <c r="B65" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C65" s="5" t="s">
+      <c r="C65" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D65" s="5" t="s">
+      <c r="D65" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E65" s="5" t="s">
+      <c r="E65" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="66" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="4" t="s">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
         <v>208</v>
       </c>
-      <c r="B66" s="5" t="s">
+      <c r="B66" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C66" s="5" t="s">
+      <c r="C66" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D66" s="5" t="s">
+      <c r="D66" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E66" s="5" t="s">
+      <c r="E66" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="67" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="4" t="s">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
         <v>209</v>
       </c>
-      <c r="B67" s="5" t="s">
+      <c r="B67" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C67" s="5" t="s">
+      <c r="C67" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D67" s="5" t="s">
+      <c r="D67" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E67" s="5" t="s">
+      <c r="E67" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="68" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="4" t="s">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
         <v>210</v>
       </c>
-      <c r="B68" s="5" t="s">
+      <c r="B68" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C68" s="5" t="s">
+      <c r="C68" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D68" s="5" t="s">
+      <c r="D68" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E68" s="5" t="s">
+      <c r="E68" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="69" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="4" t="s">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
         <v>211</v>
       </c>
-      <c r="B69" s="5" t="s">
+      <c r="B69" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C69" s="5" t="s">
+      <c r="C69" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D69" s="5" t="s">
+      <c r="D69" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E69" s="5" t="s">
+      <c r="E69" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="70" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="4" t="s">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
         <v>212</v>
       </c>
-      <c r="B70" s="5" t="s">
+      <c r="B70" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C70" s="5" t="s">
+      <c r="C70" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D70" s="5" t="s">
+      <c r="D70" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E70" s="5" t="s">
+      <c r="E70" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="71" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="4" t="s">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
         <v>213</v>
       </c>
-      <c r="B71" s="5" t="s">
+      <c r="B71" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C71" s="5" t="s">
+      <c r="C71" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D71" s="5" t="s">
+      <c r="D71" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E71" s="5" t="s">
+      <c r="E71" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="72" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="4" t="s">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
         <v>214</v>
       </c>
-      <c r="B72" s="5" t="s">
+      <c r="B72" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C72" s="5" t="s">
+      <c r="C72" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D72" s="5" t="s">
+      <c r="D72" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E72" s="5" t="s">
+      <c r="E72" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="73" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="4" t="s">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
         <v>215</v>
       </c>
-      <c r="B73" s="5" t="s">
+      <c r="B73" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C73" s="5" t="s">
+      <c r="C73" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D73" s="5" t="s">
+      <c r="D73" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E73" s="5" t="s">
+      <c r="E73" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="74" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="4" t="s">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
         <v>216</v>
       </c>
-      <c r="B74" s="5" t="s">
+      <c r="B74" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C74" s="5" t="s">
+      <c r="C74" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D74" s="5" t="s">
+      <c r="D74" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E74" s="5" t="s">
+      <c r="E74" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="75" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="4" t="s">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
         <v>217</v>
       </c>
-      <c r="B75" s="5" t="s">
+      <c r="B75" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C75" s="5" t="s">
+      <c r="C75" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D75" s="5" t="s">
+      <c r="D75" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E75" s="5" t="s">
+      <c r="E75" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="76" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="4" t="s">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
         <v>218</v>
       </c>
-      <c r="B76" s="5" t="s">
+      <c r="B76" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C76" s="5" t="s">
+      <c r="C76" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D76" s="5" t="s">
+      <c r="D76" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E76" s="5" t="s">
+      <c r="E76" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="77" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="4" t="s">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
         <v>219</v>
       </c>
-      <c r="B77" s="5" t="s">
+      <c r="B77" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C77" s="5" t="s">
+      <c r="C77" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D77" s="5" t="s">
+      <c r="D77" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E77" s="5" t="s">
+      <c r="E77" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="78" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="4" t="s">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
         <v>220</v>
       </c>
-      <c r="B78" s="5" t="s">
+      <c r="B78" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C78" s="5" t="s">
+      <c r="C78" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D78" s="5" t="s">
+      <c r="D78" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E78" s="5" t="s">
+      <c r="E78" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="79" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="4" t="s">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
         <v>221</v>
       </c>
-      <c r="B79" s="5" t="s">
+      <c r="B79" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C79" s="5" t="s">
+      <c r="C79" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D79" s="5" t="s">
+      <c r="D79" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E79" s="5" t="s">
+      <c r="E79" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="80" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="4" t="s">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
         <v>222</v>
       </c>
-      <c r="B80" s="5" t="s">
+      <c r="B80" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C80" s="5" t="s">
+      <c r="C80" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D80" s="5" t="s">
+      <c r="D80" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E80" s="5" t="s">
+      <c r="E80" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="81" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="4" t="s">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
         <v>223</v>
       </c>
-      <c r="B81" s="5" t="s">
+      <c r="B81" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C81" s="5" t="s">
+      <c r="C81" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D81" s="5" t="s">
+      <c r="D81" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E81" s="5" t="s">
+      <c r="E81" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="82" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="4" t="s">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
         <v>224</v>
       </c>
-      <c r="B82" s="5" t="s">
+      <c r="B82" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C82" s="5" t="s">
+      <c r="C82" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D82" s="5" t="s">
+      <c r="D82" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E82" s="5" t="s">
+      <c r="E82" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="83" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="4" t="s">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
         <v>225</v>
       </c>
-      <c r="B83" s="5" t="s">
+      <c r="B83" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C83" s="5" t="s">
+      <c r="C83" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D83" s="5" t="s">
+      <c r="D83" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E83" s="5" t="s">
+      <c r="E83" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="84" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="4" t="s">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
         <v>226</v>
       </c>
-      <c r="B84" s="5" t="s">
+      <c r="B84" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C84" s="5" t="s">
+      <c r="C84" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D84" s="5" t="s">
+      <c r="D84" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E84" s="5" t="s">
+      <c r="E84" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="85" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="4" t="s">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
         <v>227</v>
       </c>
-      <c r="B85" s="5" t="s">
+      <c r="B85" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C85" s="5" t="s">
+      <c r="C85" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D85" s="5" t="s">
+      <c r="D85" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E85" s="5" t="s">
+      <c r="E85" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="86" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="4" t="s">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
         <v>228</v>
       </c>
-      <c r="B86" s="5" t="s">
+      <c r="B86" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C86" s="5" t="s">
+      <c r="C86" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D86" s="5" t="s">
+      <c r="D86" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E86" s="5" t="s">
+      <c r="E86" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="87" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="4" t="s">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
         <v>229</v>
       </c>
-      <c r="B87" s="5" t="s">
+      <c r="B87" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C87" s="5" t="s">
+      <c r="C87" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D87" s="5" t="s">
+      <c r="D87" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E87" s="5" t="s">
+      <c r="E87" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="88" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="4" t="s">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
         <v>230</v>
       </c>
-      <c r="B88" s="5" t="s">
+      <c r="B88" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C88" s="5" t="s">
+      <c r="C88" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D88" s="5" t="s">
+      <c r="D88" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E88" s="5" t="s">
+      <c r="E88" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="89" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="4" t="s">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
         <v>231</v>
       </c>
-      <c r="B89" s="5" t="s">
+      <c r="B89" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C89" s="5" t="s">
+      <c r="C89" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D89" s="5" t="s">
+      <c r="D89" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E89" s="5" t="s">
+      <c r="E89" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="90" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="4" t="s">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
         <v>232</v>
       </c>
-      <c r="B90" s="5" t="s">
+      <c r="B90" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C90" s="5" t="s">
+      <c r="C90" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D90" s="5" t="s">
+      <c r="D90" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E90" s="5" t="s">
+      <c r="E90" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="91" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="4" t="s">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
         <v>233</v>
       </c>
-      <c r="B91" s="5" t="s">
+      <c r="B91" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C91" s="5" t="s">
+      <c r="C91" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D91" s="5" t="s">
+      <c r="D91" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E91" s="5" t="s">
+      <c r="E91" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="92" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="4" t="s">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
         <v>234</v>
       </c>
-      <c r="B92" s="5" t="s">
+      <c r="B92" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C92" s="5" t="s">
+      <c r="C92" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D92" s="5" t="s">
+      <c r="D92" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E92" s="5" t="s">
+      <c r="E92" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="93" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="4" t="s">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
         <v>235</v>
       </c>
-      <c r="B93" s="5" t="s">
+      <c r="B93" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C93" s="5" t="s">
+      <c r="C93" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D93" s="5" t="s">
+      <c r="D93" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E93" s="5" t="s">
+      <c r="E93" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="94" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A94" s="4" t="s">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
         <v>236</v>
       </c>
-      <c r="B94" s="5" t="s">
+      <c r="B94" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C94" s="5" t="s">
+      <c r="C94" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D94" s="5" t="s">
+      <c r="D94" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E94" s="5" t="s">
+      <c r="E94" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="95" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="4" t="s">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
         <v>237</v>
       </c>
-      <c r="B95" s="5" t="s">
+      <c r="B95" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C95" s="5" t="s">
+      <c r="C95" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D95" s="5" t="s">
+      <c r="D95" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E95" s="5" t="s">
+      <c r="E95" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="96" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="4" t="s">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
         <v>238</v>
       </c>
-      <c r="B96" s="5" t="s">
+      <c r="B96" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C96" s="5" t="s">
+      <c r="C96" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D96" s="5" t="s">
+      <c r="D96" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E96" s="5" t="s">
+      <c r="E96" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="97" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="4" t="s">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
         <v>239</v>
       </c>
-      <c r="B97" s="5" t="s">
+      <c r="B97" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C97" s="5" t="s">
+      <c r="C97" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D97" s="5" t="s">
+      <c r="D97" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E97" s="5" t="s">
+      <c r="E97" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="98" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="4" t="s">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
         <v>240</v>
       </c>
-      <c r="B98" s="5" t="s">
+      <c r="B98" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C98" s="5" t="s">
+      <c r="C98" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D98" s="5" t="s">
+      <c r="D98" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E98" s="5" t="s">
+      <c r="E98" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="99" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A99" s="4" t="s">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
         <v>241</v>
       </c>
-      <c r="B99" s="5" t="s">
+      <c r="B99" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C99" s="5" t="s">
+      <c r="C99" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D99" s="5" t="s">
+      <c r="D99" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E99" s="5" t="s">
+      <c r="E99" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="100" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A100" s="4" t="s">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
         <v>242</v>
       </c>
-      <c r="B100" s="5" t="s">
+      <c r="B100" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C100" s="5" t="s">
+      <c r="C100" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D100" s="5" t="s">
+      <c r="D100" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E100" s="5" t="s">
+      <c r="E100" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="101" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A101" s="4" t="s">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
         <v>243</v>
       </c>
-      <c r="B101" s="5" t="s">
+      <c r="B101" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C101" s="5" t="s">
+      <c r="C101" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D101" s="5" t="s">
+      <c r="D101" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E101" s="5" t="s">
+      <c r="E101" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="102" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A102" s="4" t="s">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
         <v>244</v>
       </c>
-      <c r="B102" s="5" t="s">
+      <c r="B102" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C102" s="5" t="s">
+      <c r="C102" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D102" s="5" t="s">
+      <c r="D102" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E102" s="5" t="s">
+      <c r="E102" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="103" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A103" s="4" t="s">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
         <v>245</v>
       </c>
-      <c r="B103" s="5" t="s">
+      <c r="B103" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C103" s="5" t="s">
+      <c r="C103" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D103" s="5" t="s">
+      <c r="D103" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E103" s="5" t="s">
+      <c r="E103" s="1" t="s">
         <v>40</v>
       </c>
     </row>

</xml_diff>